<commit_message>
SLD-001 added rounding, removed hardcoded 2021 year
</commit_message>
<xml_diff>
--- a/src/main/resources/EdAsStExample.xlsx
+++ b/src/main/resources/EdAsStExample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Trash\IntelliJ IDEA 2020.3.2\workspace\SLDocs\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IDEA\Idea Projects\sldocs\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F7DC39-CBC3-4E90-92E1-1E1388840D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045A2D54-B373-4B91-A6A8-FC6D398A033F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="924" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="924" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Осінь 1-3" sheetId="28" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="30">
   <si>
     <t xml:space="preserve">                        Міністерство освіти і науки  України</t>
   </si>
@@ -46,19 +46,6 @@
   </si>
   <si>
     <t>Національний технічний університет "ХПІ"</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">за кафедрою </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <rFont val="Times New Roman Cyr"/>
-      </rPr>
-      <t>ПРОГРАМНОЇ ІНЖЕНЕРІЇ ТА ІНФОРМАЦІЙНИХ ТЕХНОЛОГІЙ УПРАВЛІННЯ</t>
-    </r>
   </si>
   <si>
     <t>№ з/п</t>
@@ -134,6 +121,22 @@
   </si>
   <si>
     <t>Весна 6 курс</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">за кафедрою </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <rFont val="Times New Roman Cyr"/>
+      </rPr>
+      <t>ПРОГРАМНОЇ ІНЖЕНЕРІЇ ТА ІНТЕЛЕКТУАЛЬНИХ ТЕХНОЛОГІЙ УПРАВЛІННЯ</t>
+    </r>
+  </si>
+  <si>
+    <t>за кафедрою ПРОГРАМНОЇ ІНЖЕНЕРІЇ ТА ІНТЕЛЕКТУАЛЬНИХ ТЕХНОЛОГІЙ УПРАВЛІННЯ</t>
   </si>
 </sst>
 </file>
@@ -951,8 +954,8 @@
   </sheetPr>
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -970,7 +973,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="22.5" customHeight="1">
       <c r="A1" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -979,7 +982,7 @@
       <c r="F1" s="37"/>
       <c r="G1" s="37"/>
       <c r="H1" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
@@ -1018,7 +1021,7 @@
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -1041,7 +1044,7 @@
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="A4" s="39" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
@@ -1064,24 +1067,24 @@
     </row>
     <row r="5" spans="1:19" s="3" customFormat="1" ht="19.5" customHeight="1">
       <c r="A5" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="C5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="D5" s="44" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>7</v>
       </c>
       <c r="E5" s="45"/>
       <c r="F5" s="45"/>
       <c r="G5" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="40" t="s">
         <v>8</v>
-      </c>
-      <c r="H5" s="40" t="s">
-        <v>9</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1100,13 +1103,13 @@
       <c r="B6" s="43"/>
       <c r="C6" s="41"/>
       <c r="D6" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="F6" s="33" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>12</v>
       </c>
       <c r="G6" s="41"/>
       <c r="H6" s="41"/>
@@ -1131,7 +1134,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="19"/>
       <c r="H7" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75">
@@ -1143,7 +1146,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="19"/>
       <c r="H8" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.75">
@@ -1155,7 +1158,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="19"/>
       <c r="H9" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.75">
@@ -1167,7 +1170,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="19"/>
       <c r="H10" s="35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.75">
@@ -1179,7 +1182,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="19"/>
       <c r="H11" s="35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" ht="22.5" customHeight="1"/>
@@ -1210,8 +1213,8 @@
   </sheetPr>
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1226,7 +1229,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="6" customFormat="1" ht="18.75">
       <c r="A1" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -1235,7 +1238,7 @@
       <c r="F1" s="37"/>
       <c r="G1" s="37"/>
       <c r="H1" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" ht="18.75">
@@ -1252,7 +1255,7 @@
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -1264,7 +1267,7 @@
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="23.25" thickBot="1">
       <c r="A4" s="39" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
@@ -1276,24 +1279,24 @@
     </row>
     <row r="5" spans="1:8" s="7" customFormat="1" ht="19.5" customHeight="1">
       <c r="A5" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="C5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="D5" s="52" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>7</v>
       </c>
       <c r="E5" s="53"/>
       <c r="F5" s="53"/>
       <c r="G5" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="54" t="s">
         <v>8</v>
-      </c>
-      <c r="H5" s="54" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="7" customFormat="1" ht="42.75" customHeight="1">
@@ -1301,13 +1304,13 @@
       <c r="B6" s="49"/>
       <c r="C6" s="51"/>
       <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="51"/>
       <c r="H6" s="55"/>
@@ -1321,7 +1324,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="19"/>
       <c r="H7" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -1333,7 +1336,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="19"/>
       <c r="H8" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -1345,7 +1348,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="19"/>
       <c r="H9" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -1357,7 +1360,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="19"/>
       <c r="H10" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -1369,7 +1372,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="19"/>
       <c r="H11" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1">
@@ -1679,8 +1682,8 @@
   </sheetPr>
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1698,7 +1701,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="22.5" customHeight="1">
       <c r="A1" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -1707,7 +1710,7 @@
       <c r="F1" s="37"/>
       <c r="G1" s="37"/>
       <c r="H1" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
@@ -1746,7 +1749,7 @@
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -1769,7 +1772,7 @@
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="A4" s="39" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
@@ -1792,24 +1795,24 @@
     </row>
     <row r="5" spans="1:19" s="3" customFormat="1" ht="19.5" customHeight="1">
       <c r="A5" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="C5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="D5" s="44" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>7</v>
       </c>
       <c r="E5" s="45"/>
       <c r="F5" s="45"/>
       <c r="G5" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="40" t="s">
         <v>8</v>
-      </c>
-      <c r="H5" s="40" t="s">
-        <v>9</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1828,13 +1831,13 @@
       <c r="B6" s="43"/>
       <c r="C6" s="41"/>
       <c r="D6" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="F6" s="33" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>12</v>
       </c>
       <c r="G6" s="41"/>
       <c r="H6" s="41"/>
@@ -1859,7 +1862,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="19"/>
       <c r="H7" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75">
@@ -1871,7 +1874,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="19"/>
       <c r="H8" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.75">
@@ -1883,7 +1886,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="19"/>
       <c r="H9" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.75">
@@ -1895,7 +1898,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="19"/>
       <c r="H10" s="35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.75">
@@ -1907,7 +1910,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="19"/>
       <c r="H11" s="35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" ht="22.5" customHeight="1"/>
@@ -1938,8 +1941,8 @@
   </sheetPr>
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1954,7 +1957,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="6" customFormat="1" ht="18.75">
       <c r="A1" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -1963,7 +1966,7 @@
       <c r="F1" s="37"/>
       <c r="G1" s="37"/>
       <c r="H1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" ht="18.75">
@@ -1980,7 +1983,7 @@
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -1992,7 +1995,7 @@
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="23.25" thickBot="1">
       <c r="A4" s="39" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
@@ -2004,24 +2007,24 @@
     </row>
     <row r="5" spans="1:8" s="7" customFormat="1" ht="19.5" customHeight="1">
       <c r="A5" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="C5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="D5" s="52" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>7</v>
       </c>
       <c r="E5" s="53"/>
       <c r="F5" s="53"/>
       <c r="G5" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="54" t="s">
         <v>8</v>
-      </c>
-      <c r="H5" s="54" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="7" customFormat="1" ht="42.75" customHeight="1">
@@ -2029,13 +2032,13 @@
       <c r="B6" s="49"/>
       <c r="C6" s="51"/>
       <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="51"/>
       <c r="H6" s="55"/>
@@ -2049,7 +2052,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="19"/>
       <c r="H7" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -2061,7 +2064,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="19"/>
       <c r="H8" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -2073,7 +2076,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="19"/>
       <c r="H9" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -2085,7 +2088,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="19"/>
       <c r="H10" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -2097,7 +2100,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="19"/>
       <c r="H11" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1">
@@ -2407,8 +2410,8 @@
   </sheetPr>
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2474,7 +2477,7 @@
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" ht="30">
       <c r="A3" s="38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -2497,7 +2500,7 @@
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" ht="23.25" thickBot="1">
       <c r="A4" s="39" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
@@ -2520,24 +2523,24 @@
     </row>
     <row r="5" spans="1:19" s="3" customFormat="1" ht="15.75">
       <c r="A5" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="C5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="D5" s="52" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>7</v>
       </c>
       <c r="E5" s="53"/>
       <c r="F5" s="53"/>
       <c r="G5" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="50" t="s">
         <v>8</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>9</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -2556,13 +2559,13 @@
       <c r="B6" s="57"/>
       <c r="C6" s="51"/>
       <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>12</v>
       </c>
       <c r="G6" s="51"/>
       <c r="H6" s="51"/>
@@ -2587,7 +2590,7 @@
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
       <c r="H7" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75">
@@ -2599,7 +2602,7 @@
       <c r="F8" s="22"/>
       <c r="G8" s="23"/>
       <c r="H8" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.75">
@@ -2611,7 +2614,7 @@
       <c r="F9" s="22"/>
       <c r="G9" s="23"/>
       <c r="H9" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.75">
@@ -2623,7 +2626,7 @@
       <c r="F10" s="22"/>
       <c r="G10" s="23"/>
       <c r="H10" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.75">
@@ -2635,7 +2638,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
       <c r="H11" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2665,7 +2668,7 @@
   <dimension ref="A1:H95"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2680,7 +2683,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="6" customFormat="1" ht="18.75">
       <c r="A1" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -2689,7 +2692,7 @@
       <c r="F1" s="37"/>
       <c r="G1" s="37"/>
       <c r="H1" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" ht="18.75">
@@ -2706,7 +2709,7 @@
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -2718,7 +2721,7 @@
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="23.25" thickBot="1">
       <c r="A4" s="39" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
@@ -2730,24 +2733,24 @@
     </row>
     <row r="5" spans="1:8" s="7" customFormat="1" ht="19.5" customHeight="1">
       <c r="A5" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="C5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="D5" s="52" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>7</v>
       </c>
       <c r="E5" s="53"/>
       <c r="F5" s="53"/>
       <c r="G5" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="54" t="s">
         <v>8</v>
-      </c>
-      <c r="H5" s="54" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="7" customFormat="1" ht="42.75" customHeight="1">
@@ -2755,13 +2758,13 @@
       <c r="B6" s="49"/>
       <c r="C6" s="51"/>
       <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="51"/>
       <c r="H6" s="55"/>
@@ -2775,7 +2778,7 @@
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
       <c r="H7" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -2787,7 +2790,7 @@
       <c r="F8" s="22"/>
       <c r="G8" s="23"/>
       <c r="H8" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -2799,7 +2802,7 @@
       <c r="F9" s="22"/>
       <c r="G9" s="23"/>
       <c r="H9" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -2811,7 +2814,7 @@
       <c r="F10" s="22"/>
       <c r="G10" s="23"/>
       <c r="H10" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -2823,7 +2826,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
       <c r="H11" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1">
@@ -3167,7 +3170,7 @@
     </row>
     <row r="95" spans="3:3">
       <c r="C95" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3196,8 +3199,8 @@
   </sheetPr>
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -3215,7 +3218,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="22.5" customHeight="1">
       <c r="A1" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -3224,7 +3227,7 @@
       <c r="F1" s="37"/>
       <c r="G1" s="37"/>
       <c r="H1" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
@@ -3263,7 +3266,7 @@
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -3286,7 +3289,7 @@
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="A4" s="39" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
@@ -3309,24 +3312,24 @@
     </row>
     <row r="5" spans="1:19" s="3" customFormat="1" ht="19.5" customHeight="1">
       <c r="A5" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="C5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="D5" s="44" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>7</v>
       </c>
       <c r="E5" s="45"/>
       <c r="F5" s="45"/>
       <c r="G5" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="40" t="s">
         <v>8</v>
-      </c>
-      <c r="H5" s="40" t="s">
-        <v>9</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -3345,13 +3348,13 @@
       <c r="B6" s="43"/>
       <c r="C6" s="41"/>
       <c r="D6" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="F6" s="33" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>12</v>
       </c>
       <c r="G6" s="41"/>
       <c r="H6" s="41"/>
@@ -3376,7 +3379,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="19"/>
       <c r="H7" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75">
@@ -3388,7 +3391,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="19"/>
       <c r="H8" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.75">
@@ -3400,7 +3403,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="19"/>
       <c r="H9" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.75">
@@ -3412,7 +3415,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="19"/>
       <c r="H10" s="35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.75">
@@ -3424,7 +3427,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="19"/>
       <c r="H11" s="35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" ht="22.5" customHeight="1"/>
@@ -3455,8 +3458,8 @@
   </sheetPr>
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3471,7 +3474,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="6" customFormat="1" ht="18.75">
       <c r="A1" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -3480,7 +3483,7 @@
       <c r="F1" s="37"/>
       <c r="G1" s="37"/>
       <c r="H1" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" ht="18.75">
@@ -3497,7 +3500,7 @@
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -3509,7 +3512,7 @@
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="23.25" thickBot="1">
       <c r="A4" s="39" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
@@ -3521,24 +3524,24 @@
     </row>
     <row r="5" spans="1:8" s="7" customFormat="1" ht="19.5" customHeight="1">
       <c r="A5" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="C5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="D5" s="52" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>7</v>
       </c>
       <c r="E5" s="53"/>
       <c r="F5" s="53"/>
       <c r="G5" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="54" t="s">
         <v>8</v>
-      </c>
-      <c r="H5" s="54" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="7" customFormat="1" ht="42.75" customHeight="1">
@@ -3546,13 +3549,13 @@
       <c r="B6" s="49"/>
       <c r="C6" s="51"/>
       <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="51"/>
       <c r="H6" s="55"/>
@@ -3566,7 +3569,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="19"/>
       <c r="H7" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -3578,7 +3581,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="19"/>
       <c r="H8" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -3590,7 +3593,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="19"/>
       <c r="H9" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -3602,7 +3605,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="19"/>
       <c r="H10" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1" ht="15.75">
@@ -3614,7 +3617,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="19"/>
       <c r="H11" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1"/>

</xml_diff>